<commit_message>
Added own time recordings
</commit_message>
<xml_diff>
--- a/PM/Planning_IP-516vt_AppleTVApp4.xlsx
+++ b/PM/Planning_IP-516vt_AppleTVApp4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="444" windowWidth="23916" windowHeight="19536" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="23916" windowHeight="19536" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>Project Week</t>
   </si>
@@ -290,6 +290,24 @@
   </si>
   <si>
     <t>GUI (TVML)</t>
+  </si>
+  <si>
+    <t>Kundenmeeting + Vorbereitung</t>
+  </si>
+  <si>
+    <t>FFMpeg Research</t>
+  </si>
+  <si>
+    <t>Streaming Setup aufsetzen mit Ffmpeg und simpleHttpSever</t>
+  </si>
+  <si>
+    <t>Streaming Research JWPlayer</t>
+  </si>
+  <si>
+    <t>Streaming Research Wowza-Media-Server</t>
+  </si>
+  <si>
+    <t>Detailiertere Recherche bzgl Ffmpeg und Apple-Developer-Tools. Erstes Proof of concept</t>
   </si>
 </sst>
 </file>
@@ -1279,7 +1297,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1482,6 +1500,78 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1515,85 +1605,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2060,11 +2088,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2075,27 +2103,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="133" t="s">
+      <c r="A1" s="118" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="134"/>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
-      <c r="M1" s="134"/>
-      <c r="N1" s="134"/>
-      <c r="O1" s="134"/>
-      <c r="P1" s="134"/>
-      <c r="Q1" s="134"/>
-      <c r="R1" s="134"/>
-      <c r="S1" s="135"/>
+      <c r="B1" s="119"/>
+      <c r="C1" s="119"/>
+      <c r="D1" s="119"/>
+      <c r="E1" s="119"/>
+      <c r="F1" s="119"/>
+      <c r="G1" s="119"/>
+      <c r="H1" s="119"/>
+      <c r="I1" s="119"/>
+      <c r="J1" s="119"/>
+      <c r="K1" s="119"/>
+      <c r="L1" s="119"/>
+      <c r="M1" s="119"/>
+      <c r="N1" s="119"/>
+      <c r="O1" s="119"/>
+      <c r="P1" s="119"/>
+      <c r="Q1" s="119"/>
+      <c r="R1" s="119"/>
+      <c r="S1" s="120"/>
     </row>
     <row r="2" spans="1:23" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -2443,11 +2471,11 @@
       <c r="A14" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="142" t="s">
+      <c r="B14" s="127" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="143"/>
-      <c r="D14" s="144"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="129"/>
       <c r="E14" s="100"/>
       <c r="F14" s="101"/>
       <c r="G14" s="102" t="s">
@@ -2484,13 +2512,13 @@
       <c r="A15" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="147" t="s">
+      <c r="B15" s="134" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="148"/>
-      <c r="D15" s="148"/>
-      <c r="E15" s="148"/>
-      <c r="F15" s="149"/>
+      <c r="C15" s="135"/>
+      <c r="D15" s="135"/>
+      <c r="E15" s="135"/>
+      <c r="F15" s="136"/>
       <c r="G15" s="29">
         <v>16</v>
       </c>
@@ -2525,13 +2553,13 @@
       <c r="A16" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="121" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="137"/>
-      <c r="D16" s="137"/>
-      <c r="E16" s="137"/>
-      <c r="F16" s="138"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
+      <c r="E16" s="122"/>
+      <c r="F16" s="123"/>
       <c r="G16" s="29">
         <v>18</v>
       </c>
@@ -2552,13 +2580,13 @@
       <c r="A17" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="136" t="s">
+      <c r="B17" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="137"/>
-      <c r="D17" s="137"/>
-      <c r="E17" s="137"/>
-      <c r="F17" s="138"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122"/>
+      <c r="E17" s="122"/>
+      <c r="F17" s="123"/>
       <c r="G17" s="29">
         <v>20</v>
       </c>
@@ -2577,13 +2605,13 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="77"/>
-      <c r="B18" s="136" t="s">
+      <c r="B18" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="137"/>
-      <c r="D18" s="137"/>
-      <c r="E18" s="137"/>
-      <c r="F18" s="138"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
+      <c r="E18" s="122"/>
+      <c r="F18" s="123"/>
       <c r="G18" s="29">
         <v>14</v>
       </c>
@@ -2602,13 +2630,13 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="150" t="s">
+      <c r="B19" s="137" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="151"/>
-      <c r="D19" s="151"/>
-      <c r="E19" s="151"/>
-      <c r="F19" s="152"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="138"/>
+      <c r="F19" s="139"/>
       <c r="G19" s="29">
         <v>8</v>
       </c>
@@ -2656,13 +2684,13 @@
       <c r="A21" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="145" t="s">
+      <c r="B21" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="146"/>
-      <c r="D21" s="146"/>
-      <c r="E21" s="146"/>
-      <c r="F21" s="146"/>
+      <c r="C21" s="131"/>
+      <c r="D21" s="131"/>
+      <c r="E21" s="131"/>
+      <c r="F21" s="131"/>
       <c r="G21" s="29">
         <v>20</v>
       </c>
@@ -2695,13 +2723,13 @@
       <c r="A22" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="129" t="s">
+      <c r="B22" s="132" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
-      <c r="E22" s="130"/>
-      <c r="F22" s="130"/>
+      <c r="C22" s="133"/>
+      <c r="D22" s="133"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
       <c r="G22" s="29">
         <v>10</v>
       </c>
@@ -2720,13 +2748,13 @@
       <c r="A23" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="129" t="s">
+      <c r="B23" s="132" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="130"/>
-      <c r="D23" s="130"/>
-      <c r="E23" s="130"/>
-      <c r="F23" s="130"/>
+      <c r="C23" s="133"/>
+      <c r="D23" s="133"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
       <c r="G23" s="29">
         <v>5</v>
       </c>
@@ -2742,13 +2770,13 @@
       <c r="W23" s="31"/>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="132" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="130"/>
-      <c r="D24" s="130"/>
-      <c r="E24" s="130"/>
-      <c r="F24" s="130"/>
+      <c r="C24" s="133"/>
+      <c r="D24" s="133"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
       <c r="G24" s="29">
         <v>15</v>
       </c>
@@ -2764,13 +2792,13 @@
       <c r="W24" s="31"/>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="129" t="s">
+      <c r="B25" s="132" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="130"/>
-      <c r="D25" s="130"/>
-      <c r="E25" s="130"/>
-      <c r="F25" s="130"/>
+      <c r="C25" s="133"/>
+      <c r="D25" s="133"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
       <c r="G25" s="29">
         <v>20</v>
       </c>
@@ -2786,13 +2814,13 @@
       <c r="W25" s="31"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="129" t="s">
+      <c r="B26" s="132" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="130"/>
-      <c r="D26" s="130"/>
-      <c r="E26" s="130"/>
-      <c r="F26" s="130"/>
+      <c r="C26" s="133"/>
+      <c r="D26" s="133"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="133"/>
       <c r="G26" s="29">
         <v>15</v>
       </c>
@@ -2804,13 +2832,13 @@
       <c r="S26" s="35"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="129" t="s">
+      <c r="B27" s="132" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="130"/>
-      <c r="D27" s="130"/>
-      <c r="E27" s="130"/>
-      <c r="F27" s="130"/>
+      <c r="C27" s="133"/>
+      <c r="D27" s="133"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="133"/>
       <c r="G27" s="29">
         <v>11</v>
       </c>
@@ -2848,13 +2876,13 @@
       <c r="A29" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="131" t="s">
+      <c r="B29" s="153" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="132"/>
-      <c r="D29" s="132"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
+      <c r="C29" s="154"/>
+      <c r="D29" s="154"/>
+      <c r="E29" s="154"/>
+      <c r="F29" s="154"/>
       <c r="G29" s="29"/>
       <c r="H29" s="79"/>
       <c r="I29" s="36"/>
@@ -2873,13 +2901,13 @@
       <c r="A30" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="136" t="s">
+      <c r="B30" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="137"/>
-      <c r="D30" s="137"/>
-      <c r="E30" s="137"/>
-      <c r="F30" s="138"/>
+      <c r="C30" s="122"/>
+      <c r="D30" s="122"/>
+      <c r="E30" s="122"/>
+      <c r="F30" s="123"/>
       <c r="G30" s="29"/>
       <c r="H30" s="69"/>
       <c r="I30" s="29"/>
@@ -2901,22 +2929,22 @@
       <c r="S30" s="35"/>
     </row>
     <row r="31" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="153" t="s">
+      <c r="B31" s="140" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="154"/>
-      <c r="D31" s="154"/>
-      <c r="E31" s="154"/>
-      <c r="F31" s="154"/>
+      <c r="C31" s="141"/>
+      <c r="D31" s="141"/>
+      <c r="E31" s="141"/>
+      <c r="F31" s="141"/>
       <c r="G31" s="29"/>
       <c r="H31" s="69"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
-      <c r="M31" s="118" t="s">
+      <c r="M31" s="142" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="119"/>
-      <c r="O31" s="120"/>
+      <c r="N31" s="143"/>
+      <c r="O31" s="144"/>
       <c r="P31" s="88">
         <f>SUM(P29:P30)</f>
         <v>128</v>
@@ -2924,13 +2952,13 @@
       <c r="S31" s="35"/>
     </row>
     <row r="32" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="153" t="s">
+      <c r="B32" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="154"/>
-      <c r="D32" s="154"/>
-      <c r="E32" s="154"/>
-      <c r="F32" s="154"/>
+      <c r="C32" s="141"/>
+      <c r="D32" s="141"/>
+      <c r="E32" s="141"/>
+      <c r="F32" s="141"/>
       <c r="G32" s="29"/>
       <c r="H32" s="69"/>
       <c r="I32" s="29"/>
@@ -2943,12 +2971,12 @@
       <c r="A33" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="153" t="s">
+      <c r="B33" s="140" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="154"/>
-      <c r="D33" s="154"/>
-      <c r="E33" s="154"/>
+      <c r="C33" s="141"/>
+      <c r="D33" s="141"/>
+      <c r="E33" s="141"/>
       <c r="F33" s="155"/>
       <c r="G33" s="29"/>
       <c r="H33" s="69"/>
@@ -2959,12 +2987,12 @@
       <c r="S33" s="35"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B34" s="153" t="s">
+      <c r="B34" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="154"/>
-      <c r="D34" s="154"/>
-      <c r="E34" s="154"/>
+      <c r="C34" s="141"/>
+      <c r="D34" s="141"/>
+      <c r="E34" s="141"/>
       <c r="F34" s="155"/>
       <c r="G34" s="29"/>
       <c r="H34" s="69"/>
@@ -2975,12 +3003,12 @@
       <c r="S34" s="35"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B35" s="153" t="s">
+      <c r="B35" s="140" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="154"/>
-      <c r="D35" s="154"/>
-      <c r="E35" s="154"/>
+      <c r="C35" s="141"/>
+      <c r="D35" s="141"/>
+      <c r="E35" s="141"/>
       <c r="F35" s="155"/>
       <c r="G35" s="29"/>
       <c r="H35" s="69"/>
@@ -2994,11 +3022,11 @@
       <c r="A36" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="126"/>
-      <c r="C36" s="127"/>
-      <c r="D36" s="127"/>
-      <c r="E36" s="127"/>
-      <c r="F36" s="128"/>
+      <c r="B36" s="150"/>
+      <c r="C36" s="151"/>
+      <c r="D36" s="151"/>
+      <c r="E36" s="151"/>
+      <c r="F36" s="152"/>
       <c r="G36" s="81"/>
       <c r="H36" s="76"/>
       <c r="I36" s="38"/>
@@ -3011,11 +3039,11 @@
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="139"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="140"/>
-      <c r="E37" s="140"/>
-      <c r="F37" s="141"/>
+      <c r="B37" s="124"/>
+      <c r="C37" s="125"/>
+      <c r="D37" s="125"/>
+      <c r="E37" s="125"/>
+      <c r="F37" s="126"/>
       <c r="G37" s="81"/>
       <c r="H37" s="76"/>
       <c r="I37" s="38"/>
@@ -3049,13 +3077,13 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="92"/>
-      <c r="B39" s="121" t="s">
+      <c r="B39" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="121"/>
-      <c r="D39" s="121"/>
-      <c r="E39" s="121"/>
-      <c r="F39" s="122"/>
+      <c r="C39" s="145"/>
+      <c r="D39" s="145"/>
+      <c r="E39" s="145"/>
+      <c r="F39" s="146"/>
       <c r="G39" s="111"/>
       <c r="H39" s="94"/>
       <c r="I39" s="94"/>
@@ -3077,13 +3105,13 @@
       <c r="S39" s="93"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B40" s="136" t="s">
+      <c r="B40" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="137"/>
-      <c r="D40" s="137"/>
-      <c r="E40" s="137"/>
-      <c r="F40" s="137"/>
+      <c r="C40" s="122"/>
+      <c r="D40" s="122"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="122"/>
       <c r="G40" s="36"/>
       <c r="H40" s="79"/>
       <c r="I40" s="36"/>
@@ -3100,13 +3128,13 @@
       <c r="S40" s="35"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B41" s="136" t="s">
+      <c r="B41" s="121" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="137"/>
-      <c r="D41" s="137"/>
-      <c r="E41" s="137"/>
-      <c r="F41" s="137"/>
+      <c r="C41" s="122"/>
+      <c r="D41" s="122"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="122"/>
       <c r="G41" s="29"/>
       <c r="H41" s="69"/>
       <c r="I41" s="29"/>
@@ -3117,13 +3145,13 @@
       <c r="S41" s="35"/>
     </row>
     <row r="42" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="136" t="s">
+      <c r="B42" s="121" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="137"/>
-      <c r="D42" s="137"/>
-      <c r="E42" s="137"/>
-      <c r="F42" s="137"/>
+      <c r="C42" s="122"/>
+      <c r="D42" s="122"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="122"/>
       <c r="G42" s="38"/>
       <c r="H42" s="76"/>
       <c r="I42" s="38"/>
@@ -3145,11 +3173,11 @@
       <c r="J43" s="96"/>
       <c r="K43" s="96"/>
       <c r="L43" s="96"/>
-      <c r="M43" s="123" t="s">
+      <c r="M43" s="147" t="s">
         <v>64</v>
       </c>
-      <c r="N43" s="124"/>
-      <c r="O43" s="125"/>
+      <c r="N43" s="148"/>
+      <c r="O43" s="149"/>
       <c r="P43" s="98">
         <f>P15+P21+P29+P30+P39+P40</f>
         <v>376</v>
@@ -3244,6 +3272,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B27:F27"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="B37:F37"/>
@@ -3260,19 +3301,6 @@
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B32:F32"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3398,13 +3426,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3458,9 +3487,15 @@
         <v>4</v>
       </c>
       <c r="D5" s="40"/>
-      <c r="E5" s="115"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
+      <c r="E5" s="114">
+        <v>42664</v>
+      </c>
+      <c r="F5" s="113" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="157">
+        <v>6</v>
+      </c>
       <c r="I5" s="112"/>
       <c r="J5" s="112"/>
       <c r="K5" s="112"/>
@@ -3478,9 +3513,15 @@
         <v>6</v>
       </c>
       <c r="D6" s="40"/>
-      <c r="E6" s="115"/>
-      <c r="F6" s="113"/>
-      <c r="G6" s="113"/>
+      <c r="E6" s="156">
+        <v>42665</v>
+      </c>
+      <c r="F6" s="113" t="s">
+        <v>84</v>
+      </c>
+      <c r="G6" s="157">
+        <v>3</v>
+      </c>
       <c r="I6" s="112"/>
       <c r="J6" s="112"/>
       <c r="K6" s="112"/>
@@ -3498,9 +3539,15 @@
         <v>5</v>
       </c>
       <c r="D7" s="40"/>
-      <c r="E7" s="115"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
+      <c r="E7" s="156">
+        <v>42671</v>
+      </c>
+      <c r="F7" s="113" t="s">
+        <v>90</v>
+      </c>
+      <c r="G7" s="157">
+        <v>4</v>
+      </c>
       <c r="I7" s="112"/>
       <c r="J7" s="112"/>
       <c r="K7" s="112"/>
@@ -3518,9 +3565,15 @@
         <v>2</v>
       </c>
       <c r="D8" s="40"/>
-      <c r="E8" s="115"/>
-      <c r="F8" s="113"/>
-      <c r="G8" s="113"/>
+      <c r="E8" s="156">
+        <v>42678</v>
+      </c>
+      <c r="F8" s="113" t="s">
+        <v>89</v>
+      </c>
+      <c r="G8" s="157">
+        <v>4</v>
+      </c>
       <c r="I8" s="112"/>
       <c r="J8" s="112"/>
       <c r="K8" s="112"/>
@@ -3538,9 +3591,15 @@
         <v>2</v>
       </c>
       <c r="D9" s="40"/>
-      <c r="E9" s="115"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="113"/>
+      <c r="E9" s="156">
+        <v>42678</v>
+      </c>
+      <c r="F9" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="157">
+        <v>2</v>
+      </c>
       <c r="I9" s="112"/>
       <c r="J9" s="112"/>
       <c r="K9" s="112"/>
@@ -3558,9 +3617,15 @@
         <v>3</v>
       </c>
       <c r="D10" s="40"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
+      <c r="E10" s="156">
+        <v>42685</v>
+      </c>
+      <c r="F10" s="113" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="157">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="114">
@@ -3573,9 +3638,15 @@
         <v>2</v>
       </c>
       <c r="D11" s="40"/>
-      <c r="E11" s="115"/>
-      <c r="F11" s="113"/>
-      <c r="G11" s="113"/>
+      <c r="E11" s="156">
+        <v>42685</v>
+      </c>
+      <c r="F11" s="113" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="157">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="114">
@@ -3594,7 +3665,7 @@
       <c r="F12" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="116">
+      <c r="G12" s="157">
         <v>2</v>
       </c>
     </row>
@@ -3613,13 +3684,13 @@
         <v>42690</v>
       </c>
       <c r="F13" s="113" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+      <c r="G13" s="157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A14" s="114">
         <v>42690</v>
       </c>
@@ -3630,11 +3701,17 @@
         <v>2</v>
       </c>
       <c r="D14" s="40"/>
-      <c r="E14" s="115"/>
-      <c r="F14" s="113"/>
-      <c r="G14" s="113"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E14" s="156">
+        <v>42692</v>
+      </c>
+      <c r="F14" s="159" t="s">
+        <v>88</v>
+      </c>
+      <c r="G14" s="157">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="114">
         <v>42690</v>
       </c>
@@ -3645,11 +3722,17 @@
         <v>1</v>
       </c>
       <c r="D15" s="40"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="113"/>
-      <c r="G15" s="113"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E15" s="156">
+        <v>42693</v>
+      </c>
+      <c r="F15" s="159" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" s="157">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A16" s="114">
         <v>42692</v>
       </c>
@@ -3660,9 +3743,15 @@
         <v>4</v>
       </c>
       <c r="D16" s="40"/>
-      <c r="E16" s="115"/>
-      <c r="F16" s="113"/>
-      <c r="G16" s="113"/>
+      <c r="E16" s="156">
+        <v>42697</v>
+      </c>
+      <c r="F16" s="159" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="158">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="114">
@@ -3675,14 +3764,14 @@
         <v>1</v>
       </c>
       <c r="D17" s="40"/>
-      <c r="E17" s="114">
-        <v>42696</v>
+      <c r="E17" s="156">
+        <v>42698</v>
       </c>
       <c r="F17" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="116">
-        <v>1</v>
+      <c r="G17" s="158">
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3721,18 +3810,19 @@
       <c r="B21" s="113"/>
       <c r="C21" s="116"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="115"/>
-      <c r="F21" s="113"/>
-      <c r="G21" s="113"/>
+      <c r="F21" s="74" t="s">
+        <v>64</v>
+      </c>
+      <c r="G21">
+        <f>SUM(G5:G20)</f>
+        <v>44</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="113"/>
       <c r="B22" s="113"/>
       <c r="C22" s="116"/>
       <c r="D22" s="40"/>
-      <c r="E22" s="115"/>
-      <c r="F22" s="113"/>
-      <c r="G22" s="113"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="74" t="s">
@@ -3741,13 +3831,6 @@
       <c r="C23">
         <f>SUM(C5:C22)</f>
         <v>39</v>
-      </c>
-      <c r="F23" s="74" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23">
-        <f>SUM(G5:G22)</f>
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added project week planning
</commit_message>
<xml_diff>
--- a/PM/Planning_IP-516vt_AppleTVApp4.xlsx
+++ b/PM/Planning_IP-516vt_AppleTVApp4.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="444" windowWidth="23916" windowHeight="19536" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="444" windowWidth="23916" windowHeight="19536" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Planning" sheetId="1" r:id="rId1"/>
-    <sheet name="MileStone Definition" sheetId="2" r:id="rId2"/>
-    <sheet name="Hours_Beta" sheetId="3" r:id="rId3"/>
-    <sheet name="Hours_Gamma" sheetId="4" r:id="rId4"/>
+    <sheet name="Projectweek_Tasks" sheetId="5" r:id="rId2"/>
+    <sheet name="MileStone Definition" sheetId="2" r:id="rId3"/>
+    <sheet name="Hours_Beta" sheetId="3" r:id="rId4"/>
+    <sheet name="Hours_Gamma" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="109">
   <si>
     <t>Project Week</t>
   </si>
@@ -308,6 +309,57 @@
   </si>
   <si>
     <t>Detailiertere Recherche bzgl Ffmpeg und Apple-Developer-Tools. Erstes Proof of concept</t>
+  </si>
+  <si>
+    <t>Live-Event-Streaming</t>
+  </si>
+  <si>
+    <t>Adaptive Streaming</t>
+  </si>
+  <si>
+    <t>Encoding the variants</t>
+  </si>
+  <si>
+    <t>Keyframes</t>
+  </si>
+  <si>
+    <t>Encryption</t>
+  </si>
+  <si>
+    <t>Subtitles</t>
+  </si>
+  <si>
+    <t>Tasks Streaming</t>
+  </si>
+  <si>
+    <t>GUI/App</t>
+  </si>
+  <si>
+    <t>TV-Guide</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Est. Time</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Abstract</t>
+  </si>
+  <si>
+    <t>Streaming_Total</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>GUI/App_Total</t>
+  </si>
+  <si>
+    <t>Report_Abstract</t>
   </si>
 </sst>
 </file>
@@ -364,7 +416,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -419,8 +471,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="58">
+  <borders count="59">
     <border>
       <left/>
       <right/>
@@ -1119,6 +1177,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1297,7 +1370,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1500,120 +1573,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1624,6 +1583,121 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="175">
     <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2092,7 +2166,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2103,27 +2177,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="1" customFormat="1" ht="34.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="142" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="119"/>
-      <c r="C1" s="119"/>
-      <c r="D1" s="119"/>
-      <c r="E1" s="119"/>
-      <c r="F1" s="119"/>
-      <c r="G1" s="119"/>
-      <c r="H1" s="119"/>
-      <c r="I1" s="119"/>
-      <c r="J1" s="119"/>
-      <c r="K1" s="119"/>
-      <c r="L1" s="119"/>
-      <c r="M1" s="119"/>
-      <c r="N1" s="119"/>
-      <c r="O1" s="119"/>
-      <c r="P1" s="119"/>
-      <c r="Q1" s="119"/>
-      <c r="R1" s="119"/>
-      <c r="S1" s="120"/>
+      <c r="B1" s="143"/>
+      <c r="C1" s="143"/>
+      <c r="D1" s="143"/>
+      <c r="E1" s="143"/>
+      <c r="F1" s="143"/>
+      <c r="G1" s="143"/>
+      <c r="H1" s="143"/>
+      <c r="I1" s="143"/>
+      <c r="J1" s="143"/>
+      <c r="K1" s="143"/>
+      <c r="L1" s="143"/>
+      <c r="M1" s="143"/>
+      <c r="N1" s="143"/>
+      <c r="O1" s="143"/>
+      <c r="P1" s="143"/>
+      <c r="Q1" s="143"/>
+      <c r="R1" s="143"/>
+      <c r="S1" s="144"/>
     </row>
     <row r="2" spans="1:23" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13"/>
@@ -2471,11 +2545,11 @@
       <c r="A14" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="B14" s="127" t="s">
+      <c r="B14" s="149" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="128"/>
-      <c r="D14" s="129"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="151"/>
       <c r="E14" s="100"/>
       <c r="F14" s="101"/>
       <c r="G14" s="102" t="s">
@@ -2512,13 +2586,13 @@
       <c r="A15" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="134" t="s">
+      <c r="B15" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="135"/>
-      <c r="D15" s="135"/>
-      <c r="E15" s="135"/>
-      <c r="F15" s="136"/>
+      <c r="C15" s="155"/>
+      <c r="D15" s="155"/>
+      <c r="E15" s="155"/>
+      <c r="F15" s="156"/>
       <c r="G15" s="29">
         <v>16</v>
       </c>
@@ -2553,13 +2627,13 @@
       <c r="A16" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="121" t="s">
+      <c r="B16" s="137" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="122"/>
-      <c r="F16" s="123"/>
+      <c r="C16" s="138"/>
+      <c r="D16" s="138"/>
+      <c r="E16" s="138"/>
+      <c r="F16" s="145"/>
       <c r="G16" s="29">
         <v>18</v>
       </c>
@@ -2580,13 +2654,13 @@
       <c r="A17" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="121" t="s">
+      <c r="B17" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="122"/>
-      <c r="F17" s="123"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="138"/>
+      <c r="E17" s="138"/>
+      <c r="F17" s="145"/>
       <c r="G17" s="29">
         <v>20</v>
       </c>
@@ -2605,13 +2679,13 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="77"/>
-      <c r="B18" s="121" t="s">
+      <c r="B18" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="122"/>
-      <c r="F18" s="123"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="138"/>
+      <c r="F18" s="145"/>
       <c r="G18" s="29">
         <v>14</v>
       </c>
@@ -2630,13 +2704,13 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="79"/>
-      <c r="B19" s="137" t="s">
+      <c r="B19" s="157" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="138"/>
-      <c r="D19" s="138"/>
-      <c r="E19" s="138"/>
-      <c r="F19" s="139"/>
+      <c r="C19" s="158"/>
+      <c r="D19" s="158"/>
+      <c r="E19" s="158"/>
+      <c r="F19" s="159"/>
       <c r="G19" s="29">
         <v>8</v>
       </c>
@@ -2684,13 +2758,13 @@
       <c r="A21" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="B21" s="130" t="s">
+      <c r="B21" s="152" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="131"/>
-      <c r="D21" s="131"/>
-      <c r="E21" s="131"/>
-      <c r="F21" s="131"/>
+      <c r="C21" s="153"/>
+      <c r="D21" s="153"/>
+      <c r="E21" s="153"/>
+      <c r="F21" s="153"/>
       <c r="G21" s="29">
         <v>20</v>
       </c>
@@ -2723,13 +2797,13 @@
       <c r="A22" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="132" t="s">
+      <c r="B22" s="133" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="133"/>
-      <c r="D22" s="133"/>
-      <c r="E22" s="133"/>
-      <c r="F22" s="133"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134"/>
+      <c r="E22" s="134"/>
+      <c r="F22" s="134"/>
       <c r="G22" s="29">
         <v>10</v>
       </c>
@@ -2748,13 +2822,13 @@
       <c r="A23" s="84" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="132" t="s">
+      <c r="B23" s="133" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="133"/>
-      <c r="D23" s="133"/>
-      <c r="E23" s="133"/>
-      <c r="F23" s="133"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
+      <c r="E23" s="134"/>
+      <c r="F23" s="134"/>
       <c r="G23" s="29">
         <v>5</v>
       </c>
@@ -2770,13 +2844,13 @@
       <c r="W23" s="31"/>
     </row>
     <row r="24" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="132" t="s">
+      <c r="B24" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="133"/>
-      <c r="D24" s="133"/>
-      <c r="E24" s="133"/>
-      <c r="F24" s="133"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="134"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="134"/>
       <c r="G24" s="29">
         <v>15</v>
       </c>
@@ -2792,13 +2866,13 @@
       <c r="W24" s="31"/>
     </row>
     <row r="25" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="132" t="s">
+      <c r="B25" s="133" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="133"/>
-      <c r="D25" s="133"/>
-      <c r="E25" s="133"/>
-      <c r="F25" s="133"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134"/>
+      <c r="E25" s="134"/>
+      <c r="F25" s="134"/>
       <c r="G25" s="29">
         <v>20</v>
       </c>
@@ -2814,13 +2888,13 @@
       <c r="W25" s="31"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B26" s="132" t="s">
+      <c r="B26" s="133" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="133"/>
-      <c r="D26" s="133"/>
-      <c r="E26" s="133"/>
-      <c r="F26" s="133"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
+      <c r="F26" s="134"/>
       <c r="G26" s="29">
         <v>15</v>
       </c>
@@ -2832,13 +2906,13 @@
       <c r="S26" s="35"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="B27" s="132" t="s">
+      <c r="B27" s="133" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="133"/>
-      <c r="D27" s="133"/>
-      <c r="E27" s="133"/>
-      <c r="F27" s="133"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="134"/>
+      <c r="E27" s="134"/>
+      <c r="F27" s="134"/>
       <c r="G27" s="29">
         <v>11</v>
       </c>
@@ -2876,13 +2950,13 @@
       <c r="A29" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="153" t="s">
+      <c r="B29" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="154"/>
-      <c r="D29" s="154"/>
-      <c r="E29" s="154"/>
-      <c r="F29" s="154"/>
+      <c r="C29" s="136"/>
+      <c r="D29" s="136"/>
+      <c r="E29" s="136"/>
+      <c r="F29" s="136"/>
       <c r="G29" s="29"/>
       <c r="H29" s="79"/>
       <c r="I29" s="36"/>
@@ -2901,13 +2975,13 @@
       <c r="A30" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="121" t="s">
+      <c r="B30" s="137" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="122"/>
-      <c r="D30" s="122"/>
-      <c r="E30" s="122"/>
-      <c r="F30" s="123"/>
+      <c r="C30" s="138"/>
+      <c r="D30" s="138"/>
+      <c r="E30" s="138"/>
+      <c r="F30" s="145"/>
       <c r="G30" s="29"/>
       <c r="H30" s="69"/>
       <c r="I30" s="29"/>
@@ -2929,22 +3003,22 @@
       <c r="S30" s="35"/>
     </row>
     <row r="31" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="140" t="s">
+      <c r="B31" s="139" t="s">
         <v>30</v>
       </c>
-      <c r="C31" s="141"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="141"/>
-      <c r="F31" s="141"/>
+      <c r="C31" s="140"/>
+      <c r="D31" s="140"/>
+      <c r="E31" s="140"/>
+      <c r="F31" s="140"/>
       <c r="G31" s="29"/>
       <c r="H31" s="69"/>
       <c r="I31" s="29"/>
       <c r="J31" s="29"/>
-      <c r="M31" s="142" t="s">
+      <c r="M31" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="N31" s="143"/>
-      <c r="O31" s="144"/>
+      <c r="N31" s="123"/>
+      <c r="O31" s="124"/>
       <c r="P31" s="88">
         <f>SUM(P29:P30)</f>
         <v>128</v>
@@ -2952,13 +3026,13 @@
       <c r="S31" s="35"/>
     </row>
     <row r="32" spans="1:23" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="140" t="s">
+      <c r="B32" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="141"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="141"/>
-      <c r="F32" s="141"/>
+      <c r="C32" s="140"/>
+      <c r="D32" s="140"/>
+      <c r="E32" s="140"/>
+      <c r="F32" s="140"/>
       <c r="G32" s="29"/>
       <c r="H32" s="69"/>
       <c r="I32" s="29"/>
@@ -2971,13 +3045,13 @@
       <c r="A33" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B33" s="140" t="s">
+      <c r="B33" s="139" t="s">
         <v>32</v>
       </c>
-      <c r="C33" s="141"/>
-      <c r="D33" s="141"/>
-      <c r="E33" s="141"/>
-      <c r="F33" s="155"/>
+      <c r="C33" s="140"/>
+      <c r="D33" s="140"/>
+      <c r="E33" s="140"/>
+      <c r="F33" s="141"/>
       <c r="G33" s="29"/>
       <c r="H33" s="69"/>
       <c r="I33" s="29"/>
@@ -2987,13 +3061,13 @@
       <c r="S33" s="35"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B34" s="140" t="s">
+      <c r="B34" s="139" t="s">
         <v>33</v>
       </c>
-      <c r="C34" s="141"/>
-      <c r="D34" s="141"/>
-      <c r="E34" s="141"/>
-      <c r="F34" s="155"/>
+      <c r="C34" s="140"/>
+      <c r="D34" s="140"/>
+      <c r="E34" s="140"/>
+      <c r="F34" s="141"/>
       <c r="G34" s="29"/>
       <c r="H34" s="69"/>
       <c r="I34" s="29"/>
@@ -3003,13 +3077,13 @@
       <c r="S34" s="35"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B35" s="140" t="s">
+      <c r="B35" s="139" t="s">
         <v>34</v>
       </c>
-      <c r="C35" s="141"/>
-      <c r="D35" s="141"/>
-      <c r="E35" s="141"/>
-      <c r="F35" s="155"/>
+      <c r="C35" s="140"/>
+      <c r="D35" s="140"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="141"/>
       <c r="G35" s="29"/>
       <c r="H35" s="69"/>
       <c r="I35" s="29"/>
@@ -3022,11 +3096,11 @@
       <c r="A36" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="150"/>
-      <c r="C36" s="151"/>
-      <c r="D36" s="151"/>
-      <c r="E36" s="151"/>
-      <c r="F36" s="152"/>
+      <c r="B36" s="130"/>
+      <c r="C36" s="131"/>
+      <c r="D36" s="131"/>
+      <c r="E36" s="131"/>
+      <c r="F36" s="132"/>
       <c r="G36" s="81"/>
       <c r="H36" s="76"/>
       <c r="I36" s="38"/>
@@ -3039,11 +3113,11 @@
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="124"/>
-      <c r="C37" s="125"/>
-      <c r="D37" s="125"/>
-      <c r="E37" s="125"/>
-      <c r="F37" s="126"/>
+      <c r="B37" s="146"/>
+      <c r="C37" s="147"/>
+      <c r="D37" s="147"/>
+      <c r="E37" s="147"/>
+      <c r="F37" s="148"/>
       <c r="G37" s="81"/>
       <c r="H37" s="76"/>
       <c r="I37" s="38"/>
@@ -3077,13 +3151,13 @@
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="92"/>
-      <c r="B39" s="145" t="s">
+      <c r="B39" s="125" t="s">
         <v>80</v>
       </c>
-      <c r="C39" s="145"/>
-      <c r="D39" s="145"/>
-      <c r="E39" s="145"/>
-      <c r="F39" s="146"/>
+      <c r="C39" s="125"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="125"/>
+      <c r="F39" s="126"/>
       <c r="G39" s="111"/>
       <c r="H39" s="94"/>
       <c r="I39" s="94"/>
@@ -3105,13 +3179,13 @@
       <c r="S39" s="93"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B40" s="121" t="s">
+      <c r="B40" s="137" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="122"/>
-      <c r="D40" s="122"/>
-      <c r="E40" s="122"/>
-      <c r="F40" s="122"/>
+      <c r="C40" s="138"/>
+      <c r="D40" s="138"/>
+      <c r="E40" s="138"/>
+      <c r="F40" s="138"/>
       <c r="G40" s="36"/>
       <c r="H40" s="79"/>
       <c r="I40" s="36"/>
@@ -3128,13 +3202,13 @@
       <c r="S40" s="35"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B41" s="121" t="s">
+      <c r="B41" s="137" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="122"/>
-      <c r="D41" s="122"/>
-      <c r="E41" s="122"/>
-      <c r="F41" s="122"/>
+      <c r="C41" s="138"/>
+      <c r="D41" s="138"/>
+      <c r="E41" s="138"/>
+      <c r="F41" s="138"/>
       <c r="G41" s="29"/>
       <c r="H41" s="69"/>
       <c r="I41" s="29"/>
@@ -3145,13 +3219,13 @@
       <c r="S41" s="35"/>
     </row>
     <row r="42" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="122"/>
-      <c r="D42" s="122"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="122"/>
+      <c r="C42" s="138"/>
+      <c r="D42" s="138"/>
+      <c r="E42" s="138"/>
+      <c r="F42" s="138"/>
       <c r="G42" s="38"/>
       <c r="H42" s="76"/>
       <c r="I42" s="38"/>
@@ -3173,11 +3247,11 @@
       <c r="J43" s="96"/>
       <c r="K43" s="96"/>
       <c r="L43" s="96"/>
-      <c r="M43" s="147" t="s">
+      <c r="M43" s="127" t="s">
         <v>64</v>
       </c>
-      <c r="N43" s="148"/>
-      <c r="O43" s="149"/>
+      <c r="N43" s="128"/>
+      <c r="O43" s="129"/>
       <c r="P43" s="98">
         <f>P15+P21+P29+P30+P39+P40</f>
         <v>376</v>
@@ -3272,19 +3346,6 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B27:F27"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="B30:F30"/>
     <mergeCell ref="B37:F37"/>
@@ -3301,6 +3362,19 @@
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="B31:F31"/>
     <mergeCell ref="B32:F32"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B27:F27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3309,10 +3383,176 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="160" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="160" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B2:B8)</f>
+        <v>41</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B10:B14)</f>
+        <v>44</v>
+      </c>
+      <c r="H2">
+        <f>B17</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="160" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="160" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>104</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -3422,11 +3662,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3493,7 +3733,7 @@
       <c r="F5" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="157">
+      <c r="G5" s="119">
         <v>6</v>
       </c>
       <c r="I5" s="112"/>
@@ -3513,13 +3753,13 @@
         <v>6</v>
       </c>
       <c r="D6" s="40"/>
-      <c r="E6" s="156">
+      <c r="E6" s="118">
         <v>42665</v>
       </c>
       <c r="F6" s="113" t="s">
         <v>84</v>
       </c>
-      <c r="G6" s="157">
+      <c r="G6" s="119">
         <v>3</v>
       </c>
       <c r="I6" s="112"/>
@@ -3539,13 +3779,13 @@
         <v>5</v>
       </c>
       <c r="D7" s="40"/>
-      <c r="E7" s="156">
+      <c r="E7" s="118">
         <v>42671</v>
       </c>
       <c r="F7" s="113" t="s">
         <v>90</v>
       </c>
-      <c r="G7" s="157">
+      <c r="G7" s="119">
         <v>4</v>
       </c>
       <c r="I7" s="112"/>
@@ -3565,13 +3805,13 @@
         <v>2</v>
       </c>
       <c r="D8" s="40"/>
-      <c r="E8" s="156">
+      <c r="E8" s="118">
         <v>42678</v>
       </c>
       <c r="F8" s="113" t="s">
         <v>89</v>
       </c>
-      <c r="G8" s="157">
+      <c r="G8" s="119">
         <v>4</v>
       </c>
       <c r="I8" s="112"/>
@@ -3591,13 +3831,13 @@
         <v>2</v>
       </c>
       <c r="D9" s="40"/>
-      <c r="E9" s="156">
+      <c r="E9" s="118">
         <v>42678</v>
       </c>
       <c r="F9" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="157">
+      <c r="G9" s="119">
         <v>2</v>
       </c>
       <c r="I9" s="112"/>
@@ -3617,13 +3857,13 @@
         <v>3</v>
       </c>
       <c r="D10" s="40"/>
-      <c r="E10" s="156">
+      <c r="E10" s="118">
         <v>42685</v>
       </c>
       <c r="F10" s="113" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="157">
+      <c r="G10" s="119">
         <v>2</v>
       </c>
     </row>
@@ -3638,13 +3878,13 @@
         <v>2</v>
       </c>
       <c r="D11" s="40"/>
-      <c r="E11" s="156">
+      <c r="E11" s="118">
         <v>42685</v>
       </c>
       <c r="F11" s="113" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="157">
+      <c r="G11" s="119">
         <v>3</v>
       </c>
     </row>
@@ -3665,7 +3905,7 @@
       <c r="F12" s="113" t="s">
         <v>82</v>
       </c>
-      <c r="G12" s="157">
+      <c r="G12" s="119">
         <v>2</v>
       </c>
     </row>
@@ -3686,7 +3926,7 @@
       <c r="F13" s="113" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="157">
+      <c r="G13" s="119">
         <v>2</v>
       </c>
     </row>
@@ -3701,13 +3941,13 @@
         <v>2</v>
       </c>
       <c r="D14" s="40"/>
-      <c r="E14" s="156">
+      <c r="E14" s="118">
         <v>42692</v>
       </c>
-      <c r="F14" s="159" t="s">
+      <c r="F14" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="157">
+      <c r="G14" s="119">
         <v>5</v>
       </c>
     </row>
@@ -3722,13 +3962,13 @@
         <v>1</v>
       </c>
       <c r="D15" s="40"/>
-      <c r="E15" s="156">
+      <c r="E15" s="118">
         <v>42693</v>
       </c>
-      <c r="F15" s="159" t="s">
+      <c r="F15" s="121" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="157">
+      <c r="G15" s="119">
         <v>4</v>
       </c>
     </row>
@@ -3743,13 +3983,13 @@
         <v>4</v>
       </c>
       <c r="D16" s="40"/>
-      <c r="E16" s="156">
+      <c r="E16" s="118">
         <v>42697</v>
       </c>
-      <c r="F16" s="159" t="s">
+      <c r="F16" s="121" t="s">
         <v>91</v>
       </c>
-      <c r="G16" s="158">
+      <c r="G16" s="120">
         <v>5</v>
       </c>
     </row>
@@ -3764,13 +4004,13 @@
         <v>1</v>
       </c>
       <c r="D17" s="40"/>
-      <c r="E17" s="156">
+      <c r="E17" s="118">
         <v>42698</v>
       </c>
       <c r="F17" s="113" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="158">
+      <c r="G17" s="120">
         <v>2</v>
       </c>
     </row>
@@ -3838,7 +4078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G46"/>
   <sheetViews>

</xml_diff>